<commit_message>
shiny created, linelist exported
</commit_message>
<xml_diff>
--- a/linelist_FATE_raw.xlsx
+++ b/linelist_FATE_raw.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\edvtempfs.krhs.hbg.zsanbw.de\homes$\10086038\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alena\Documents\Digital Health GitHub Projects\FATE\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE5F99B1-F598-4ECF-88B2-EC10F37FC7B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -21,12 +22,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Milena Braun</author>
   </authors>
   <commentList>
-    <comment ref="N27" authorId="0" shapeId="0">
+    <comment ref="N27" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -55,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="281">
   <si>
     <t>FATE Patientenevaluation</t>
   </si>
@@ -886,12 +887,24 @@
   </si>
   <si>
     <t>Auswertung (deskriptiv)</t>
+  </si>
+  <si>
+    <t>correct</t>
+  </si>
+  <si>
+    <t>false neg</t>
+  </si>
+  <si>
+    <t>false pos</t>
+  </si>
+  <si>
+    <t>error_type</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -968,7 +981,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -1108,6 +1121,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1163,16 +1196,12 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1188,9 +1217,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1228,9 +1257,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1265,7 +1294,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1300,7 +1329,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1473,37 +1502,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P112"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:R112"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD6"/>
+    <sheetView tabSelected="1" topLeftCell="M11" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="J44" sqref="J44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="2"/>
-    <col min="2" max="2" width="35.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="11.42578125" style="1"/>
-    <col min="7" max="7" width="11.42578125" style="18"/>
-    <col min="8" max="8" width="17.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="43.85546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="59.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="70.85546875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="32.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" style="2"/>
+    <col min="2" max="2" width="35.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="11.44140625" style="1"/>
+    <col min="7" max="7" width="11.44140625" style="18"/>
+    <col min="8" max="8" width="17.88671875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="43.88671875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="59.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="70.88671875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="32.5546875" style="2" customWidth="1"/>
     <col min="14" max="14" width="9" style="2" customWidth="1"/>
-    <col min="15" max="15" width="113.5703125" style="2" customWidth="1"/>
-    <col min="16" max="16384" width="11.42578125" style="2"/>
+    <col min="15" max="15" width="113.5546875" style="2" customWidth="1"/>
+    <col min="16" max="17" width="9.33203125" style="2" customWidth="1"/>
+    <col min="18" max="16384" width="11.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
@@ -1546,8 +1576,14 @@
       <c r="O4" s="3" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P4" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -1590,11 +1626,15 @@
       <c r="O5" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="P5" s="3">
+      <c r="P5" s="15">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -1637,11 +1677,15 @@
       <c r="O6" s="15" t="s">
         <v>174</v>
       </c>
-      <c r="P6" s="3">
+      <c r="P6" s="15">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -1684,11 +1728,15 @@
       <c r="O7" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="P7" s="3">
+      <c r="P7" s="15">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1731,11 +1779,15 @@
       <c r="O8" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="P8" s="3">
+      <c r="P8" s="15">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="3">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>9</v>
       </c>
@@ -1778,11 +1830,15 @@
       <c r="O9" s="15" t="s">
         <v>178</v>
       </c>
-      <c r="P9" s="3">
+      <c r="P9" s="15">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="3">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>10</v>
       </c>
@@ -1825,11 +1881,15 @@
       <c r="O10" s="15" t="s">
         <v>179</v>
       </c>
-      <c r="P10" s="3">
+      <c r="P10" s="15">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="15"/>
+      <c r="R10" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>11</v>
       </c>
@@ -1872,11 +1932,15 @@
       <c r="O11" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="P11" s="3">
+      <c r="P11" s="15">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="3">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>15</v>
       </c>
@@ -1919,11 +1983,17 @@
       <c r="O12" s="16" t="s">
         <v>180</v>
       </c>
-      <c r="P12" s="3">
+      <c r="P12" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="16" t="s">
+        <v>279</v>
+      </c>
+      <c r="R12" s="3">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>17</v>
       </c>
@@ -1969,11 +2039,15 @@
       <c r="O13" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="P13" s="3">
+      <c r="P13" s="15">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="3">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>18</v>
       </c>
@@ -2019,11 +2093,15 @@
       <c r="O14" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="P14" s="3">
+      <c r="P14" s="15">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="15"/>
+      <c r="R14" s="3">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>22</v>
       </c>
@@ -2069,11 +2147,15 @@
       <c r="O15" s="15" t="s">
         <v>182</v>
       </c>
-      <c r="P15" s="3">
+      <c r="P15" s="15">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="15"/>
+      <c r="R15" s="3">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>27</v>
       </c>
@@ -2119,11 +2201,17 @@
       <c r="O16" s="16" t="s">
         <v>184</v>
       </c>
-      <c r="P16" s="3">
+      <c r="P16" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="16" t="s">
+        <v>278</v>
+      </c>
+      <c r="R16" s="3">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>28</v>
       </c>
@@ -2169,11 +2257,15 @@
       <c r="O17" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="P17" s="3">
+      <c r="P17" s="15">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="15"/>
+      <c r="R17" s="3">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>29</v>
       </c>
@@ -2219,11 +2311,17 @@
       <c r="O18" s="16" t="s">
         <v>186</v>
       </c>
-      <c r="P18" s="3">
+      <c r="P18" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="16" t="s">
+        <v>279</v>
+      </c>
+      <c r="R18" s="3">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>30</v>
       </c>
@@ -2269,11 +2367,17 @@
       <c r="O19" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="P19" s="3">
+      <c r="P19" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="16" t="s">
+        <v>279</v>
+      </c>
+      <c r="R19" s="3">
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>33</v>
       </c>
@@ -2319,11 +2423,17 @@
       <c r="O20" s="16" t="s">
         <v>188</v>
       </c>
-      <c r="P20" s="3">
+      <c r="P20" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="16" t="s">
+        <v>279</v>
+      </c>
+      <c r="R20" s="3">
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>34</v>
       </c>
@@ -2369,11 +2479,17 @@
       <c r="O21" s="16" t="s">
         <v>189</v>
       </c>
-      <c r="P21" s="3">
+      <c r="P21" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="16" t="s">
+        <v>279</v>
+      </c>
+      <c r="R21" s="3">
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>37</v>
       </c>
@@ -2419,11 +2535,15 @@
       <c r="O22" s="15" t="s">
         <v>190</v>
       </c>
-      <c r="P22" s="3">
+      <c r="P22" s="15">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="15"/>
+      <c r="R22" s="3">
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>38</v>
       </c>
@@ -2469,11 +2589,17 @@
       <c r="O23" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="P23" s="3">
+      <c r="P23" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="16" t="s">
+        <v>279</v>
+      </c>
+      <c r="R23" s="3">
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>42</v>
       </c>
@@ -2516,11 +2642,17 @@
       <c r="O24" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="P24" s="3">
+      <c r="P24" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="16" t="s">
+        <v>279</v>
+      </c>
+      <c r="R24" s="3">
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>43</v>
       </c>
@@ -2563,11 +2695,15 @@
       <c r="O25" s="15" t="s">
         <v>191</v>
       </c>
-      <c r="P25" s="3">
+      <c r="P25" s="15">
+        <v>1</v>
+      </c>
+      <c r="Q25" s="15"/>
+      <c r="R25" s="3">
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>44</v>
       </c>
@@ -2613,11 +2749,15 @@
       <c r="O26" s="15" t="s">
         <v>192</v>
       </c>
-      <c r="P26" s="3">
+      <c r="P26" s="15">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="15"/>
+      <c r="R26" s="3">
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>47</v>
       </c>
@@ -2660,11 +2800,17 @@
       <c r="O27" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="P27" s="3">
+      <c r="P27" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="16" t="s">
+        <v>279</v>
+      </c>
+      <c r="R27" s="3">
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>52</v>
       </c>
@@ -2707,11 +2853,15 @@
       <c r="O28" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="P28" s="3">
+      <c r="P28" s="15">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="15"/>
+      <c r="R28" s="3">
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>54</v>
       </c>
@@ -2757,11 +2907,17 @@
       <c r="O29" s="16" t="s">
         <v>194</v>
       </c>
-      <c r="P29" s="3">
+      <c r="P29" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="16" t="s">
+        <v>278</v>
+      </c>
+      <c r="R29" s="3">
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>56</v>
       </c>
@@ -2807,11 +2963,15 @@
       <c r="O30" s="15" t="s">
         <v>195</v>
       </c>
-      <c r="P30" s="3">
+      <c r="P30" s="15">
+        <v>1</v>
+      </c>
+      <c r="Q30" s="15"/>
+      <c r="R30" s="3">
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>57</v>
       </c>
@@ -2857,11 +3017,15 @@
       <c r="O31" s="15" t="s">
         <v>195</v>
       </c>
-      <c r="P31" s="3">
+      <c r="P31" s="15">
+        <v>1</v>
+      </c>
+      <c r="Q31" s="15"/>
+      <c r="R31" s="3">
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>58</v>
       </c>
@@ -2907,11 +3071,15 @@
       <c r="O32" s="15" t="s">
         <v>196</v>
       </c>
-      <c r="P32" s="3">
+      <c r="P32" s="15">
+        <v>1</v>
+      </c>
+      <c r="Q32" s="15"/>
+      <c r="R32" s="3">
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>60</v>
       </c>
@@ -2957,11 +3125,15 @@
       <c r="O33" s="15" t="s">
         <v>198</v>
       </c>
-      <c r="P33" s="3">
+      <c r="P33" s="15">
+        <v>1</v>
+      </c>
+      <c r="Q33" s="15"/>
+      <c r="R33" s="3">
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>62</v>
       </c>
@@ -3007,11 +3179,15 @@
       <c r="O34" s="15" t="s">
         <v>199</v>
       </c>
-      <c r="P34" s="3">
+      <c r="P34" s="15">
+        <v>1</v>
+      </c>
+      <c r="Q34" s="15"/>
+      <c r="R34" s="3">
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>67</v>
       </c>
@@ -3057,11 +3233,15 @@
       <c r="O35" s="15" t="s">
         <v>200</v>
       </c>
-      <c r="P35" s="3">
+      <c r="P35" s="15">
+        <v>1</v>
+      </c>
+      <c r="Q35" s="15"/>
+      <c r="R35" s="3">
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>72</v>
       </c>
@@ -3107,11 +3287,15 @@
       <c r="O36" s="15" t="s">
         <v>201</v>
       </c>
-      <c r="P36" s="3">
+      <c r="P36" s="15">
+        <v>1</v>
+      </c>
+      <c r="Q36" s="15"/>
+      <c r="R36" s="3">
         <v>72</v>
       </c>
     </row>
-    <row r="37" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>74</v>
       </c>
@@ -3154,11 +3338,17 @@
       <c r="O37" s="16" t="s">
         <v>202</v>
       </c>
-      <c r="P37" s="3">
+      <c r="P37" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q37" s="16" t="s">
+        <v>278</v>
+      </c>
+      <c r="R37" s="3">
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>77</v>
       </c>
@@ -3204,11 +3394,15 @@
       <c r="O38" s="15" t="s">
         <v>203</v>
       </c>
-      <c r="P38" s="3">
+      <c r="P38" s="15">
+        <v>1</v>
+      </c>
+      <c r="Q38" s="15"/>
+      <c r="R38" s="3">
         <v>77</v>
       </c>
     </row>
-    <row r="39" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>80</v>
       </c>
@@ -3254,11 +3448,15 @@
       <c r="O39" s="15" t="s">
         <v>204</v>
       </c>
-      <c r="P39" s="3">
+      <c r="P39" s="15">
+        <v>1</v>
+      </c>
+      <c r="Q39" s="15"/>
+      <c r="R39" s="3">
         <v>80</v>
       </c>
     </row>
-    <row r="40" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
         <v>81</v>
       </c>
@@ -3304,11 +3502,15 @@
       <c r="O40" s="17" t="s">
         <v>205</v>
       </c>
-      <c r="P40" s="3">
+      <c r="P40" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q40" s="17"/>
+      <c r="R40" s="3">
         <v>81</v>
       </c>
     </row>
-    <row r="41" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <v>82</v>
       </c>
@@ -3354,11 +3556,15 @@
       <c r="O41" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="P41" s="3">
+      <c r="P41" s="15">
+        <v>1</v>
+      </c>
+      <c r="Q41" s="15"/>
+      <c r="R41" s="3">
         <v>82</v>
       </c>
     </row>
-    <row r="42" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
         <v>85</v>
       </c>
@@ -3404,11 +3610,15 @@
       <c r="O42" s="15" t="s">
         <v>206</v>
       </c>
-      <c r="P42" s="3">
+      <c r="P42" s="15">
+        <v>1</v>
+      </c>
+      <c r="Q42" s="15"/>
+      <c r="R42" s="3">
         <v>85</v>
       </c>
     </row>
-    <row r="43" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <v>87</v>
       </c>
@@ -3454,11 +3664,17 @@
       <c r="O43" s="16" t="s">
         <v>207</v>
       </c>
-      <c r="P43" s="3">
+      <c r="P43" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q43" s="16" t="s">
+        <v>278</v>
+      </c>
+      <c r="R43" s="3">
         <v>87</v>
       </c>
     </row>
-    <row r="44" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
         <v>94</v>
       </c>
@@ -3504,11 +3720,15 @@
       <c r="O44" s="15" t="s">
         <v>208</v>
       </c>
-      <c r="P44" s="3">
+      <c r="P44" s="15">
+        <v>1</v>
+      </c>
+      <c r="Q44" s="15"/>
+      <c r="R44" s="3">
         <v>94</v>
       </c>
     </row>
-    <row r="45" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="5">
         <v>95</v>
       </c>
@@ -3522,7 +3742,7 @@
       <c r="K45" s="6"/>
       <c r="L45" s="6"/>
     </row>
-    <row r="46" spans="1:16" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:18" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="5">
         <v>96</v>
       </c>
@@ -3545,8 +3765,10 @@
         <v>229</v>
       </c>
       <c r="O46" s="9"/>
-    </row>
-    <row r="47" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P46" s="9"/>
+      <c r="Q46" s="9"/>
+    </row>
+    <row r="47" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="5">
         <v>97</v>
       </c>
@@ -3569,9 +3791,11 @@
       <c r="O47" s="11" t="s">
         <v>209</v>
       </c>
-      <c r="P47" s="8"/>
-    </row>
-    <row r="48" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P47" s="23"/>
+      <c r="Q47" s="23"/>
+      <c r="R47" s="8"/>
+    </row>
+    <row r="48" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="5">
         <v>98</v>
       </c>
@@ -3594,9 +3818,11 @@
       <c r="O48" s="12" t="s">
         <v>210</v>
       </c>
-      <c r="P48" s="8"/>
-    </row>
-    <row r="49" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P48" s="29"/>
+      <c r="Q48" s="29"/>
+      <c r="R48" s="8"/>
+    </row>
+    <row r="49" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="5">
         <v>99</v>
       </c>
@@ -3621,9 +3847,11 @@
       <c r="O49" s="12" t="s">
         <v>211</v>
       </c>
-      <c r="P49" s="8"/>
-    </row>
-    <row r="50" spans="1:16" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P49" s="29"/>
+      <c r="Q49" s="29"/>
+      <c r="R49" s="8"/>
+    </row>
+    <row r="50" spans="1:18" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="5">
         <v>100</v>
       </c>
@@ -3646,9 +3874,11 @@
       <c r="O50" s="13" t="s">
         <v>212</v>
       </c>
-      <c r="P50" s="8"/>
-    </row>
-    <row r="51" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P50" s="30"/>
+      <c r="Q50" s="30"/>
+      <c r="R50" s="8"/>
+    </row>
+    <row r="51" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="5">
         <v>101</v>
       </c>
@@ -3666,38 +3896,40 @@
       <c r="K51" s="6"/>
       <c r="L51" s="6"/>
       <c r="O51" s="10"/>
-    </row>
-    <row r="52" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P51" s="10"/>
+      <c r="Q51" s="10"/>
+    </row>
+    <row r="52" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="9"/>
       <c r="B52" s="9"/>
       <c r="C52" s="9"/>
       <c r="D52" s="22"/>
       <c r="E52" s="26"/>
-      <c r="F52" s="28"/>
-      <c r="G52" s="29"/>
-      <c r="H52" s="28"/>
-      <c r="I52" s="28"/>
-      <c r="J52" s="28"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="18"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+      <c r="J52" s="1"/>
       <c r="K52" s="21"/>
       <c r="L52" s="6"/>
     </row>
-    <row r="53" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="2"/>
-      <c r="B53" s="30" t="s">
+      <c r="B53" s="28" t="s">
         <v>276</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
-      <c r="F53" s="28"/>
-      <c r="G53" s="29"/>
-      <c r="H53" s="28"/>
-      <c r="I53" s="28"/>
-      <c r="J53" s="28"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="18"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
       <c r="K53" s="21"/>
       <c r="L53" s="6"/>
     </row>
-    <row r="54" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2"/>
       <c r="B54" s="2" t="s">
         <v>236</v>
@@ -3705,29 +3937,29 @@
       <c r="C54" s="2"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
-      <c r="F54" s="28"/>
-      <c r="G54" s="29"/>
-      <c r="H54" s="28"/>
-      <c r="I54" s="28"/>
-      <c r="J54" s="28"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="18"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
       <c r="K54" s="21"/>
       <c r="L54" s="6"/>
     </row>
-    <row r="55" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
-      <c r="F55" s="28"/>
-      <c r="G55" s="29"/>
-      <c r="H55" s="28"/>
-      <c r="I55" s="28"/>
-      <c r="J55" s="28"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="18"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
+      <c r="J55" s="1"/>
       <c r="K55" s="21"/>
       <c r="L55" s="6"/>
     </row>
-    <row r="56" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="2"/>
       <c r="B56" s="2" t="s">
         <v>237</v>
@@ -3737,15 +3969,15 @@
       </c>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
-      <c r="F56" s="28"/>
-      <c r="G56" s="29"/>
-      <c r="H56" s="28"/>
-      <c r="I56" s="28"/>
-      <c r="J56" s="28"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="18"/>
+      <c r="H56" s="1"/>
+      <c r="I56" s="1"/>
+      <c r="J56" s="1"/>
       <c r="K56" s="21"/>
       <c r="L56" s="6"/>
     </row>
-    <row r="57" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="2"/>
       <c r="B57" s="23" t="s">
         <v>238</v>
@@ -3753,15 +3985,15 @@
       <c r="C57" s="23"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
-      <c r="F57" s="28"/>
-      <c r="G57" s="29"/>
-      <c r="H57" s="28"/>
-      <c r="I57" s="28"/>
-      <c r="J57" s="28"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="18"/>
+      <c r="H57" s="1"/>
+      <c r="I57" s="1"/>
+      <c r="J57" s="1"/>
       <c r="K57" s="21"/>
       <c r="L57" s="6"/>
     </row>
-    <row r="58" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="2"/>
       <c r="B58" s="2" t="s">
         <v>239</v>
@@ -3771,15 +4003,15 @@
       </c>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
-      <c r="F58" s="28"/>
-      <c r="G58" s="29"/>
-      <c r="H58" s="28"/>
-      <c r="I58" s="28"/>
-      <c r="J58" s="28"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="18"/>
+      <c r="H58" s="1"/>
+      <c r="I58" s="1"/>
+      <c r="J58" s="1"/>
       <c r="K58" s="21"/>
       <c r="L58" s="6"/>
     </row>
-    <row r="59" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="2"/>
       <c r="B59" s="2" t="s">
         <v>240</v>
@@ -3789,29 +4021,29 @@
       </c>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
-      <c r="F59" s="28"/>
-      <c r="G59" s="29"/>
-      <c r="H59" s="28"/>
-      <c r="I59" s="28"/>
-      <c r="J59" s="28"/>
+      <c r="F59" s="1"/>
+      <c r="G59" s="18"/>
+      <c r="H59" s="1"/>
+      <c r="I59" s="1"/>
+      <c r="J59" s="1"/>
       <c r="K59" s="21"/>
       <c r="L59" s="6"/>
     </row>
-    <row r="60" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
-      <c r="F60" s="28"/>
-      <c r="G60" s="29"/>
-      <c r="H60" s="28"/>
-      <c r="I60" s="28"/>
-      <c r="J60" s="28"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="18"/>
+      <c r="H60" s="1"/>
+      <c r="I60" s="1"/>
+      <c r="J60" s="1"/>
       <c r="K60" s="21"/>
       <c r="L60" s="6"/>
     </row>
-    <row r="61" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2"/>
       <c r="B61" s="23" t="s">
         <v>241</v>
@@ -3819,15 +4051,15 @@
       <c r="C61" s="23"/>
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
-      <c r="F61" s="28"/>
-      <c r="G61" s="29"/>
-      <c r="H61" s="28"/>
-      <c r="I61" s="28"/>
-      <c r="J61" s="28"/>
+      <c r="F61" s="1"/>
+      <c r="G61" s="18"/>
+      <c r="H61" s="1"/>
+      <c r="I61" s="1"/>
+      <c r="J61" s="1"/>
       <c r="K61" s="21"/>
       <c r="L61" s="6"/>
     </row>
-    <row r="62" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2"/>
       <c r="B62" s="2" t="s">
         <v>244</v>
@@ -3837,15 +4069,15 @@
       </c>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
-      <c r="F62" s="28"/>
-      <c r="G62" s="29"/>
-      <c r="H62" s="28"/>
-      <c r="I62" s="28"/>
-      <c r="J62" s="28"/>
+      <c r="F62" s="1"/>
+      <c r="G62" s="18"/>
+      <c r="H62" s="1"/>
+      <c r="I62" s="1"/>
+      <c r="J62" s="1"/>
       <c r="K62" s="21"/>
       <c r="L62" s="6"/>
     </row>
-    <row r="63" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="2"/>
       <c r="B63" s="2" t="s">
         <v>242</v>
@@ -3855,15 +4087,15 @@
       </c>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
-      <c r="F63" s="28"/>
-      <c r="G63" s="29"/>
-      <c r="H63" s="28"/>
-      <c r="I63" s="28"/>
-      <c r="J63" s="28"/>
+      <c r="F63" s="1"/>
+      <c r="G63" s="18"/>
+      <c r="H63" s="1"/>
+      <c r="I63" s="1"/>
+      <c r="J63" s="1"/>
       <c r="K63" s="21"/>
       <c r="L63" s="6"/>
     </row>
-    <row r="64" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="2"/>
       <c r="B64" s="2" t="s">
         <v>243</v>
@@ -3873,29 +4105,29 @@
       </c>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
-      <c r="F64" s="28"/>
-      <c r="G64" s="29"/>
-      <c r="H64" s="28"/>
-      <c r="I64" s="28"/>
-      <c r="J64" s="28"/>
+      <c r="F64" s="1"/>
+      <c r="G64" s="18"/>
+      <c r="H64" s="1"/>
+      <c r="I64" s="1"/>
+      <c r="J64" s="1"/>
       <c r="K64" s="21"/>
       <c r="L64" s="6"/>
     </row>
-    <row r="65" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
-      <c r="F65" s="28"/>
-      <c r="G65" s="29"/>
-      <c r="H65" s="28"/>
-      <c r="I65" s="28"/>
-      <c r="J65" s="28"/>
+      <c r="F65" s="1"/>
+      <c r="G65" s="18"/>
+      <c r="H65" s="1"/>
+      <c r="I65" s="1"/>
+      <c r="J65" s="1"/>
       <c r="K65" s="21"/>
       <c r="L65" s="6"/>
     </row>
-    <row r="66" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A66" s="2"/>
       <c r="B66" s="23" t="s">
         <v>264</v>
@@ -3903,15 +4135,15 @@
       <c r="C66" s="23"/>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
-      <c r="F66" s="28"/>
-      <c r="G66" s="29"/>
-      <c r="H66" s="28"/>
-      <c r="I66" s="28"/>
-      <c r="J66" s="28"/>
+      <c r="F66" s="1"/>
+      <c r="G66" s="18"/>
+      <c r="H66" s="1"/>
+      <c r="I66" s="1"/>
+      <c r="J66" s="1"/>
       <c r="K66" s="21"/>
       <c r="L66" s="6"/>
     </row>
-    <row r="67" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A67" s="2"/>
       <c r="B67" s="2" t="s">
         <v>233</v>
@@ -3921,15 +4153,15 @@
       </c>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
-      <c r="F67" s="28"/>
-      <c r="G67" s="29"/>
-      <c r="H67" s="28"/>
-      <c r="I67" s="28"/>
-      <c r="J67" s="28"/>
+      <c r="F67" s="1"/>
+      <c r="G67" s="18"/>
+      <c r="H67" s="1"/>
+      <c r="I67" s="1"/>
+      <c r="J67" s="1"/>
       <c r="K67" s="21"/>
       <c r="L67" s="6"/>
     </row>
-    <row r="68" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A68" s="2"/>
       <c r="B68" s="2" t="s">
         <v>234</v>
@@ -3939,15 +4171,15 @@
       </c>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
-      <c r="F68" s="28"/>
-      <c r="G68" s="29"/>
-      <c r="H68" s="28"/>
-      <c r="I68" s="28"/>
-      <c r="J68" s="28"/>
+      <c r="F68" s="1"/>
+      <c r="G68" s="18"/>
+      <c r="H68" s="1"/>
+      <c r="I68" s="1"/>
+      <c r="J68" s="1"/>
       <c r="K68" s="21"/>
       <c r="L68" s="6"/>
     </row>
-    <row r="69" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="2"/>
       <c r="B69" s="2" t="s">
         <v>235</v>
@@ -3957,29 +4189,29 @@
       </c>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
-      <c r="F69" s="28"/>
-      <c r="G69" s="29"/>
-      <c r="H69" s="28"/>
-      <c r="I69" s="28"/>
-      <c r="J69" s="28"/>
+      <c r="F69" s="1"/>
+      <c r="G69" s="18"/>
+      <c r="H69" s="1"/>
+      <c r="I69" s="1"/>
+      <c r="J69" s="1"/>
       <c r="K69" s="21"/>
       <c r="L69" s="6"/>
     </row>
-    <row r="70" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
-      <c r="F70" s="28"/>
-      <c r="G70" s="29"/>
-      <c r="H70" s="28"/>
-      <c r="I70" s="28"/>
-      <c r="J70" s="28"/>
+      <c r="F70" s="1"/>
+      <c r="G70" s="18"/>
+      <c r="H70" s="1"/>
+      <c r="I70" s="1"/>
+      <c r="J70" s="1"/>
       <c r="K70" s="21"/>
       <c r="L70" s="6"/>
     </row>
-    <row r="71" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A71" s="2"/>
       <c r="B71" s="23" t="s">
         <v>245</v>
@@ -3987,15 +4219,15 @@
       <c r="C71" s="23"/>
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
-      <c r="F71" s="28"/>
-      <c r="G71" s="29"/>
-      <c r="H71" s="28"/>
-      <c r="I71" s="28"/>
-      <c r="J71" s="28"/>
+      <c r="F71" s="1"/>
+      <c r="G71" s="18"/>
+      <c r="H71" s="1"/>
+      <c r="I71" s="1"/>
+      <c r="J71" s="1"/>
       <c r="K71" s="21"/>
       <c r="L71" s="6"/>
     </row>
-    <row r="72" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A72" s="2"/>
       <c r="B72" s="2" t="s">
         <v>255</v>
@@ -4005,16 +4237,16 @@
       </c>
       <c r="D72" s="2"/>
       <c r="E72" s="1"/>
-      <c r="F72" s="28"/>
-      <c r="G72" s="28"/>
-      <c r="H72" s="29"/>
-      <c r="I72" s="28"/>
-      <c r="J72" s="28"/>
+      <c r="F72" s="1"/>
+      <c r="G72" s="1"/>
+      <c r="H72" s="18"/>
+      <c r="I72" s="1"/>
+      <c r="J72" s="1"/>
       <c r="K72" s="21"/>
       <c r="L72" s="6"/>
       <c r="M72" s="6"/>
     </row>
-    <row r="73" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A73" s="2"/>
       <c r="B73" s="2" t="s">
         <v>256</v>
@@ -4024,16 +4256,16 @@
       </c>
       <c r="D73" s="2"/>
       <c r="E73" s="1"/>
-      <c r="F73" s="28"/>
-      <c r="G73" s="28"/>
-      <c r="H73" s="29"/>
-      <c r="I73" s="28"/>
-      <c r="J73" s="28"/>
+      <c r="F73" s="1"/>
+      <c r="G73" s="1"/>
+      <c r="H73" s="18"/>
+      <c r="I73" s="1"/>
+      <c r="J73" s="1"/>
       <c r="K73" s="21"/>
       <c r="L73" s="6"/>
       <c r="M73" s="6"/>
     </row>
-    <row r="74" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74" s="2"/>
       <c r="B74" s="2" t="s">
         <v>257</v>
@@ -4043,31 +4275,31 @@
       </c>
       <c r="D74" s="2"/>
       <c r="E74" s="1"/>
-      <c r="F74" s="28"/>
-      <c r="G74" s="28"/>
-      <c r="H74" s="29"/>
-      <c r="I74" s="28"/>
-      <c r="J74" s="28"/>
+      <c r="F74" s="1"/>
+      <c r="G74" s="1"/>
+      <c r="H74" s="18"/>
+      <c r="I74" s="1"/>
+      <c r="J74" s="1"/>
       <c r="K74" s="21"/>
       <c r="L74" s="6"/>
       <c r="M74" s="6"/>
     </row>
-    <row r="75" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
       <c r="E75" s="1"/>
-      <c r="F75" s="28"/>
-      <c r="G75" s="28"/>
-      <c r="H75" s="29"/>
-      <c r="I75" s="28"/>
-      <c r="J75" s="28"/>
+      <c r="F75" s="1"/>
+      <c r="G75" s="1"/>
+      <c r="H75" s="18"/>
+      <c r="I75" s="1"/>
+      <c r="J75" s="1"/>
       <c r="K75" s="21"/>
       <c r="L75" s="6"/>
       <c r="M75" s="6"/>
     </row>
-    <row r="76" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A76" s="2"/>
       <c r="B76" s="23" t="s">
         <v>254</v>
@@ -4075,15 +4307,15 @@
       <c r="C76" s="23"/>
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
-      <c r="F76" s="28"/>
-      <c r="G76" s="29"/>
-      <c r="H76" s="28"/>
-      <c r="I76" s="28"/>
-      <c r="J76" s="28"/>
+      <c r="F76" s="1"/>
+      <c r="G76" s="18"/>
+      <c r="H76" s="1"/>
+      <c r="I76" s="1"/>
+      <c r="J76" s="1"/>
       <c r="K76" s="21"/>
       <c r="L76" s="6"/>
     </row>
-    <row r="77" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A77" s="2"/>
       <c r="B77" s="2" t="s">
         <v>246</v>
@@ -4093,15 +4325,15 @@
       </c>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
-      <c r="F77" s="28"/>
-      <c r="G77" s="29"/>
-      <c r="H77" s="28"/>
-      <c r="I77" s="28"/>
-      <c r="J77" s="28"/>
+      <c r="F77" s="1"/>
+      <c r="G77" s="18"/>
+      <c r="H77" s="1"/>
+      <c r="I77" s="1"/>
+      <c r="J77" s="1"/>
       <c r="K77" s="21"/>
       <c r="L77" s="6"/>
     </row>
-    <row r="78" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A78" s="2"/>
       <c r="B78" s="2" t="s">
         <v>247</v>
@@ -4111,15 +4343,15 @@
       </c>
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
-      <c r="F78" s="28"/>
-      <c r="G78" s="29"/>
-      <c r="H78" s="28"/>
-      <c r="I78" s="28"/>
-      <c r="J78" s="28"/>
+      <c r="F78" s="1"/>
+      <c r="G78" s="18"/>
+      <c r="H78" s="1"/>
+      <c r="I78" s="1"/>
+      <c r="J78" s="1"/>
       <c r="K78" s="21"/>
       <c r="L78" s="6"/>
     </row>
-    <row r="79" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A79" s="2"/>
       <c r="B79" s="2" t="s">
         <v>248</v>
@@ -4129,29 +4361,29 @@
       </c>
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
-      <c r="F79" s="28"/>
-      <c r="G79" s="29"/>
-      <c r="H79" s="28"/>
-      <c r="I79" s="28"/>
-      <c r="J79" s="28"/>
+      <c r="F79" s="1"/>
+      <c r="G79" s="18"/>
+      <c r="H79" s="1"/>
+      <c r="I79" s="1"/>
+      <c r="J79" s="1"/>
       <c r="K79" s="21"/>
       <c r="L79" s="6"/>
     </row>
-    <row r="80" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
       <c r="D80" s="1"/>
       <c r="E80" s="1"/>
-      <c r="F80" s="28"/>
-      <c r="G80" s="29"/>
-      <c r="H80" s="28"/>
-      <c r="I80" s="28"/>
-      <c r="J80" s="28"/>
+      <c r="F80" s="1"/>
+      <c r="G80" s="18"/>
+      <c r="H80" s="1"/>
+      <c r="I80" s="1"/>
+      <c r="J80" s="1"/>
       <c r="K80" s="21"/>
       <c r="L80" s="6"/>
     </row>
-    <row r="81" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A81" s="2"/>
       <c r="B81" s="23" t="s">
         <v>274</v>
@@ -4159,15 +4391,15 @@
       <c r="C81" s="25"/>
       <c r="D81" s="1"/>
       <c r="E81" s="1"/>
-      <c r="F81" s="28"/>
-      <c r="G81" s="29"/>
-      <c r="H81" s="28"/>
-      <c r="I81" s="28"/>
-      <c r="J81" s="28"/>
+      <c r="F81" s="1"/>
+      <c r="G81" s="18"/>
+      <c r="H81" s="1"/>
+      <c r="I81" s="1"/>
+      <c r="J81" s="1"/>
       <c r="K81" s="21"/>
       <c r="L81" s="6"/>
     </row>
-    <row r="82" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A82" s="2"/>
       <c r="B82" s="2" t="s">
         <v>265</v>
@@ -4177,15 +4409,15 @@
       </c>
       <c r="D82" s="1"/>
       <c r="E82" s="1"/>
-      <c r="F82" s="28"/>
-      <c r="G82" s="29"/>
-      <c r="H82" s="28"/>
-      <c r="I82" s="28"/>
-      <c r="J82" s="28"/>
+      <c r="F82" s="1"/>
+      <c r="G82" s="18"/>
+      <c r="H82" s="1"/>
+      <c r="I82" s="1"/>
+      <c r="J82" s="1"/>
       <c r="K82" s="21"/>
       <c r="L82" s="6"/>
     </row>
-    <row r="83" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A83" s="2"/>
       <c r="B83" s="2" t="s">
         <v>266</v>
@@ -4195,28 +4427,23 @@
       </c>
       <c r="D83" s="1"/>
       <c r="E83" s="1"/>
-      <c r="F83" s="28"/>
-      <c r="G83" s="29"/>
-      <c r="H83" s="28"/>
-      <c r="I83" s="28"/>
-      <c r="J83" s="28"/>
+      <c r="F83" s="1"/>
+      <c r="G83" s="18"/>
+      <c r="H83" s="1"/>
+      <c r="I83" s="1"/>
+      <c r="J83" s="1"/>
       <c r="K83" s="21"/>
       <c r="L83" s="6"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B84" s="2" t="s">
         <v>267</v>
       </c>
       <c r="C84" s="24">
         <v>9</v>
       </c>
-      <c r="F84" s="28"/>
-      <c r="G84" s="29"/>
-      <c r="H84" s="28"/>
-      <c r="I84" s="28"/>
-      <c r="J84" s="28"/>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B85" s="2" t="s">
         <v>268</v>
       </c>
@@ -4224,7 +4451,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B87" s="2" t="s">
         <v>269</v>
       </c>
@@ -4232,7 +4459,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B88" s="2" t="s">
         <v>270</v>
       </c>
@@ -4240,12 +4467,12 @@
         <v>251</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C96" s="2" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="110" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C110" s="2" t="s">
         <v>21</v>
       </c>
@@ -4271,7 +4498,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="111" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C111" s="2" t="s">
         <v>24</v>
       </c>
@@ -4297,7 +4524,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="112" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C112" s="2" t="s">
         <v>28</v>
       </c>
@@ -4331,24 +4558,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>